<commit_message>
added application battery, intent, keycapture tests to selendroid
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/System_Ruby.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/System_Ruby.xlsx
@@ -75,9 +75,6 @@
     <t>Navigate to Google</t>
   </si>
   <si>
-    <t>System-JS</t>
-  </si>
-  <si>
     <t>call getProperty with country</t>
   </si>
   <si>
@@ -604,6 +601,9 @@
 {
 validate_SystemProperties=getallproperties
 };</t>
+  </si>
+  <si>
+    <t>System-Ruby</t>
   </si>
 </sst>
 </file>
@@ -1084,7 +1084,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1139,22 +1139,22 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="F2" s="9">
         <v>1</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>10</v>
@@ -1171,19 +1171,19 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="9">
         <v>1</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="2"/>
@@ -1198,19 +1198,19 @@
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="9">
         <v>1</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="2"/>
@@ -1225,7 +1225,7 @@
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>11</v>
@@ -1234,10 +1234,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
@@ -1252,7 +1252,7 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>12</v>
@@ -1261,10 +1261,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
@@ -1279,7 +1279,7 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>13</v>
@@ -1288,10 +1288,10 @@
         <v>1</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
@@ -1306,19 +1306,19 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8" s="9">
         <v>1</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>14</v>
@@ -1342,10 +1342,10 @@
         <v>1</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
@@ -1360,7 +1360,7 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>15</v>
@@ -1369,10 +1369,10 @@
         <v>1</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>16</v>
@@ -1396,10 +1396,10 @@
         <v>1</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
@@ -1414,19 +1414,19 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F12" s="9">
         <v>1</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
@@ -1441,19 +1441,19 @@
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F13" s="9">
         <v>1</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
@@ -1468,19 +1468,19 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F14" s="9">
         <v>1</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
@@ -1495,19 +1495,19 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" s="9">
         <v>1</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
@@ -1522,19 +1522,19 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F16" s="9">
         <v>1</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
@@ -1549,7 +1549,7 @@
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>17</v>
@@ -1558,10 +1558,10 @@
         <v>1</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>

</xml_diff>